<commit_message>
The Label class works
</commit_message>
<xml_diff>
--- a/Characters/Characters.xlsx
+++ b/Characters/Characters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="143">
   <si>
     <t>Array</t>
   </si>
@@ -843,8 +843,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="265">
+  <cellStyleXfs count="279">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1334,7 +1348,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="265">
+  <cellStyles count="279">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -1467,6 +1481,13 @@
     <cellStyle name="Collegamento ipertestuale" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="277" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -1599,6 +1620,13 @@
     <cellStyle name="Collegamento visitato" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="278" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="87">
@@ -2976,7 +3004,7 @@
   <dimension ref="B1:DX279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D5" sqref="D5:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3123,9 +3151,8 @@
         <v>0x61</v>
       </c>
       <c r="D5" s="61" t="str">
-        <f ca="1">IF(ISBLANK(E5)," ",
-"static const uint8_t   " &amp; (INDIRECT("'"&amp;E5&amp;"'!W"&amp;(VALUE(F5)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E5&amp;"'!X"&amp;(VALUE(F5)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E5&amp;"'!X"&amp;(VALUE(F5)+4))&amp;" , "&amp;INDIRECT("'"&amp;E5&amp;"'!Y"&amp;(VALUE(F5)+4))&amp;"};")</f>
-        <v>static const uint8_t   a   [6] = { 5 , 0x20, 0x54, 0x54, 0x54, 0x38};</v>
+        <f ca="1">IF(ISBLANK(E5)," ","static const PROGMEM uint8_t   " &amp; (INDIRECT("'"&amp;E5&amp;"'!W"&amp;(VALUE(F5)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E5&amp;"'!X"&amp;(VALUE(F5)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E5&amp;"'!X"&amp;(VALUE(F5)+4))&amp;" , "&amp;INDIRECT("'"&amp;E5&amp;"'!Y"&amp;(VALUE(F5)+4))&amp;"};")</f>
+        <v>static const PROGMEM uint8_t   a   [5] = { 4 , 0x24, 0x54, 0x54, 0x78};</v>
       </c>
       <c r="E5" s="59" t="s">
         <v>64</v>
@@ -3150,9 +3177,8 @@
         <v>0x62</v>
       </c>
       <c r="D6" s="61" t="str">
-        <f t="shared" ref="D6:D69" ca="1" si="1">IF(ISBLANK(E6)," ",
-"static const uint8_t   " &amp; (INDIRECT("'"&amp;E6&amp;"'!W"&amp;(VALUE(F6)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E6&amp;"'!X"&amp;(VALUE(F6)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E6&amp;"'!X"&amp;(VALUE(F6)+4))&amp;" , "&amp;INDIRECT("'"&amp;E6&amp;"'!Y"&amp;(VALUE(F6)+4))&amp;"};")</f>
-        <v>static const uint8_t   b   [5] = { 4 , 0x7E, 0x44, 0x44, 0x38};</v>
+        <f t="shared" ref="D6:D69" ca="1" si="1">IF(ISBLANK(E6)," ","static const PROGMEM uint8_t   " &amp; (INDIRECT("'"&amp;E6&amp;"'!W"&amp;(VALUE(F6)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E6&amp;"'!X"&amp;(VALUE(F6)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E6&amp;"'!X"&amp;(VALUE(F6)+4))&amp;" , "&amp;INDIRECT("'"&amp;E6&amp;"'!Y"&amp;(VALUE(F6)+4))&amp;"};")</f>
+        <v>static const PROGMEM uint8_t   b   [5] = { 4 , 0x7E, 0x44, 0x44, 0x38};</v>
       </c>
       <c r="E6" s="59" t="s">
         <v>64</v>
@@ -3178,7 +3204,7 @@
       </c>
       <c r="D7" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   c   [5] = { 4 , 0x38, 0x44, 0x44, 0x44};</v>
+        <v>static const PROGMEM uint8_t   c   [5] = { 4 , 0x38, 0x44, 0x44, 0x44};</v>
       </c>
       <c r="E7" s="59" t="s">
         <v>64</v>
@@ -3205,7 +3231,7 @@
       </c>
       <c r="D8" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   d   [5] = { 4 , 0x30, 0x48, 0x48, 0x7E};</v>
+        <v>static const PROGMEM uint8_t   d   [5] = { 4 , 0x38, 0x44, 0x44, 0x7E};</v>
       </c>
       <c r="E8" s="59" t="s">
         <v>64</v>
@@ -3231,7 +3257,7 @@
       </c>
       <c r="D9" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   e   [5] = { 4 , 0x38, 0x54, 0x54, 0x08};</v>
+        <v>static const PROGMEM uint8_t   e   [5] = { 4 , 0x38, 0x54, 0x54, 0x08};</v>
       </c>
       <c r="E9" s="59" t="s">
         <v>64</v>
@@ -3257,7 +3283,7 @@
       </c>
       <c r="D10" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   f   [5] = { 4 , 0x08, 0x7C, 0xA, 0x02};</v>
+        <v>static const PROGMEM uint8_t   f   [5] = { 4 , 0x08, 0x7C, 0xA, 0x02};</v>
       </c>
       <c r="E10" s="59" t="s">
         <v>64</v>
@@ -3283,7 +3309,7 @@
       </c>
       <c r="D11" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   g   [5] = { 4 , 0x18, 0xA4, 0xA4, 0x7C};</v>
+        <v>static const PROGMEM uint8_t   g   [5] = { 4 , 0x18, 0xA4, 0xA4, 0x7C};</v>
       </c>
       <c r="E11" s="59" t="s">
         <v>64</v>
@@ -3309,7 +3335,7 @@
       </c>
       <c r="D12" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   h   [5] = { 4 , 0x7E, 0x04, 0x04, 0x78};</v>
+        <v>static const PROGMEM uint8_t   h   [5] = { 4 , 0x7E, 0x04, 0x04, 0x78};</v>
       </c>
       <c r="E12" s="59" t="s">
         <v>64</v>
@@ -3335,7 +3361,7 @@
       </c>
       <c r="D13" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   i   [2] = { 1 , 0x7D};</v>
+        <v>static const PROGMEM uint8_t   i   [2] = { 1 , 0x7D};</v>
       </c>
       <c r="E13" s="59" t="s">
         <v>64</v>
@@ -3361,7 +3387,7 @@
       </c>
       <c r="D14" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   j   [3] = { 2 , 0x80, 0x7D};</v>
+        <v>static const PROGMEM uint8_t   j   [3] = { 2 , 0x80, 0x7D};</v>
       </c>
       <c r="E14" s="59" t="s">
         <v>64</v>
@@ -3387,7 +3413,7 @@
       </c>
       <c r="D15" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   k   [4] = { 3 , 0x7E, 0x10, 0x68};</v>
+        <v>static const PROGMEM uint8_t   k   [4] = { 3 , 0x7E, 0x10, 0x68};</v>
       </c>
       <c r="E15" s="59" t="s">
         <v>64</v>
@@ -3413,7 +3439,7 @@
       </c>
       <c r="D16" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   l   [2] = { 1 , 0x7E};</v>
+        <v>static const PROGMEM uint8_t   l   [2] = { 1 , 0x7E};</v>
       </c>
       <c r="E16" s="59" t="s">
         <v>64</v>
@@ -3439,7 +3465,7 @@
       </c>
       <c r="D17" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   m   [8] = { 7 , 0x7C, 0x04, 0x04, 0x78, 0x04, 0x04, 0x78};</v>
+        <v>static const PROGMEM uint8_t   m   [8] = { 7 , 0x7C, 0x04, 0x04, 0x78, 0x04, 0x04, 0x78};</v>
       </c>
       <c r="E17" s="59" t="s">
         <v>64</v>
@@ -3465,7 +3491,7 @@
       </c>
       <c r="D18" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   n   [5] = { 4 , 0x7C, 0x04, 0x04, 0x78};</v>
+        <v>static const PROGMEM uint8_t   n   [5] = { 4 , 0x7C, 0x04, 0x04, 0x78};</v>
       </c>
       <c r="E18" s="59" t="s">
         <v>64</v>
@@ -3491,7 +3517,7 @@
       </c>
       <c r="D19" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   o   [5] = { 4 , 0x38, 0x44, 0x44, 0x38};</v>
+        <v>static const PROGMEM uint8_t   o   [5] = { 4 , 0x38, 0x44, 0x44, 0x38};</v>
       </c>
       <c r="E19" s="59" t="s">
         <v>64</v>
@@ -3517,7 +3543,7 @@
       </c>
       <c r="D20" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   p   [5] = { 4 , 0xFC, 0x44, 0x44, 0x38};</v>
+        <v>static const PROGMEM uint8_t   p   [5] = { 4 , 0xFC, 0x44, 0x44, 0x38};</v>
       </c>
       <c r="E20" s="59" t="s">
         <v>64</v>
@@ -3543,7 +3569,7 @@
       </c>
       <c r="D21" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   q   [5] = { 4 , 0x38, 0x44, 0x44, 0xFC};</v>
+        <v>static const PROGMEM uint8_t   q   [5] = { 4 , 0x38, 0x44, 0x44, 0xFC};</v>
       </c>
       <c r="E21" s="59" t="s">
         <v>64</v>
@@ -3569,7 +3595,7 @@
       </c>
       <c r="D22" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   r   [4] = { 3 , 0x7C, 0x08, 0x04};</v>
+        <v>static const PROGMEM uint8_t   r   [4] = { 3 , 0x7C, 0x08, 0x04};</v>
       </c>
       <c r="E22" s="59" t="s">
         <v>64</v>
@@ -3595,7 +3621,7 @@
       </c>
       <c r="D23" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   s   [4] = { 3 , 0x5C, 0x54, 0x74};</v>
+        <v>static const PROGMEM uint8_t   s   [4] = { 3 , 0x58, 0x54, 0x34};</v>
       </c>
       <c r="E23" s="59" t="s">
         <v>64</v>
@@ -3621,7 +3647,7 @@
       </c>
       <c r="D24" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   t   [4] = { 3 , 0x04, 0x3E, 0x44};</v>
+        <v>static const PROGMEM uint8_t   t   [4] = { 3 , 0x04, 0x3E, 0x44};</v>
       </c>
       <c r="E24" s="59" t="s">
         <v>64</v>
@@ -3647,7 +3673,7 @@
       </c>
       <c r="D25" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   u   [5] = { 4 , 0x3C, 0x40, 0x40, 0x7C};</v>
+        <v>static const PROGMEM uint8_t   u   [5] = { 4 , 0x3C, 0x40, 0x40, 0x7C};</v>
       </c>
       <c r="E25" s="59" t="s">
         <v>64</v>
@@ -3673,7 +3699,7 @@
       </c>
       <c r="D26" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   v   [6] = { 5 , 0xC, 0x30, 0x40, 0x30, 0xC};</v>
+        <v>static const PROGMEM uint8_t   v   [6] = { 5 , 0xC, 0x30, 0x40, 0x30, 0xC};</v>
       </c>
       <c r="E26" s="59" t="s">
         <v>64</v>
@@ -3699,7 +3725,7 @@
       </c>
       <c r="D27" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   w   [6] = { 5 , 0x3C, 0x40, 0x20, 0x40, 0x3C};</v>
+        <v>static const PROGMEM uint8_t   w   [6] = { 5 , 0x3C, 0x40, 0x20, 0x40, 0x3C};</v>
       </c>
       <c r="E27" s="59" t="s">
         <v>64</v>
@@ -3725,7 +3751,7 @@
       </c>
       <c r="D28" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   x   [6] = { 5 , 0x44, 0x28, 0x10, 0x28, 0x44};</v>
+        <v>static const PROGMEM uint8_t   x   [6] = { 5 , 0x44, 0x28, 0x10, 0x28, 0x44};</v>
       </c>
       <c r="E28" s="59" t="s">
         <v>64</v>
@@ -3751,7 +3777,7 @@
       </c>
       <c r="D29" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   y   [5] = { 4 , 0xC, 0x50, 0x30, 0xC};</v>
+        <v>static const PROGMEM uint8_t   y   [5] = { 4 , 0xC, 0x50, 0x30, 0xC};</v>
       </c>
       <c r="E29" s="59" t="s">
         <v>64</v>
@@ -3777,7 +3803,7 @@
       </c>
       <c r="D30" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   z   [5] = { 4 , 0x64, 0x54, 0x54, 0x4C};</v>
+        <v>static const PROGMEM uint8_t   z   [5] = { 4 , 0x64, 0x54, 0x54, 0x4C};</v>
       </c>
       <c r="E30" s="59" t="s">
         <v>64</v>
@@ -3818,7 +3844,7 @@
       </c>
       <c r="D32" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   A   [6] = { 5 , 0x7E, 0x09, 0x09, 0x09, 0x7E};</v>
+        <v>static const PROGMEM uint8_t   A   [6] = { 5 , 0x7E, 0x09, 0x09, 0x09, 0x7E};</v>
       </c>
       <c r="E32" s="55" t="s">
         <v>126</v>
@@ -3844,7 +3870,7 @@
       </c>
       <c r="D33" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   B   [5] = { 4 , 0x7F, 0x49, 0x49, 0x36};</v>
+        <v>static const PROGMEM uint8_t   B   [5] = { 4 , 0x7F, 0x49, 0x49, 0x36};</v>
       </c>
       <c r="E33" s="55" t="s">
         <v>126</v>
@@ -3870,7 +3896,7 @@
       </c>
       <c r="D34" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   C   [5] = { 4 , 0x3E, 0x41, 0x41, 0x41};</v>
+        <v>static const PROGMEM uint8_t   C   [5] = { 4 , 0x3E, 0x41, 0x41, 0x41};</v>
       </c>
       <c r="E34" s="55" t="s">
         <v>126</v>
@@ -3896,7 +3922,7 @@
       </c>
       <c r="D35" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   D   [5] = { 4 , 0x7F, 0x41, 0x22, 0x1C};</v>
+        <v>static const PROGMEM uint8_t   D   [5] = { 4 , 0x7F, 0x41, 0x22, 0x1C};</v>
       </c>
       <c r="E35" s="55" t="s">
         <v>126</v>
@@ -3922,7 +3948,7 @@
       </c>
       <c r="D36" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   E   [5] = { 4 , 0x7F, 0x49, 0x49, 0x41};</v>
+        <v>static const PROGMEM uint8_t   E   [5] = { 4 , 0x7F, 0x49, 0x49, 0x41};</v>
       </c>
       <c r="E36" s="55" t="s">
         <v>126</v>
@@ -3948,7 +3974,7 @@
       </c>
       <c r="D37" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   F   [5] = { 4 , 0x7F, 0x05, 0x05, 0x01};</v>
+        <v>static const PROGMEM uint8_t   F   [5] = { 4 , 0x7F, 0x05, 0x05, 0x01};</v>
       </c>
       <c r="E37" s="55" t="s">
         <v>126</v>
@@ -3974,7 +4000,7 @@
       </c>
       <c r="D38" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   G   [6] = { 5 , 0x3E, 0x41, 0x49, 0x49, 0x39};</v>
+        <v>static const PROGMEM uint8_t   G   [6] = { 5 , 0x3E, 0x41, 0x49, 0x49, 0x39};</v>
       </c>
       <c r="E38" s="55" t="s">
         <v>126</v>
@@ -4000,7 +4026,7 @@
       </c>
       <c r="D39" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   H   [6] = { 5 , 0x7F, 0x08, 0x08, 0x08, 0x7F};</v>
+        <v>static const PROGMEM uint8_t   H   [6] = { 5 , 0x7F, 0x08, 0x08, 0x08, 0x7F};</v>
       </c>
       <c r="E39" s="55" t="s">
         <v>126</v>
@@ -4026,7 +4052,7 @@
       </c>
       <c r="D40" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   I   [2] = { 1 , 0x7F};</v>
+        <v>static const PROGMEM uint8_t   I   [2] = { 1 , 0x7F};</v>
       </c>
       <c r="E40" s="55" t="s">
         <v>126</v>
@@ -4052,7 +4078,7 @@
       </c>
       <c r="D41" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   J   [4] = { 3 , 0x60, 0x40, 0x7F};</v>
+        <v>static const PROGMEM uint8_t   J   [4] = { 3 , 0x60, 0x40, 0x7F};</v>
       </c>
       <c r="E41" s="55" t="s">
         <v>126</v>
@@ -4078,7 +4104,7 @@
       </c>
       <c r="D42" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   K   [5] = { 4 , 0x7F, 0xC, 0x12, 0x61};</v>
+        <v>static const PROGMEM uint8_t   K   [5] = { 4 , 0x7F, 0xC, 0x12, 0x61};</v>
       </c>
       <c r="E42" s="55" t="s">
         <v>126</v>
@@ -4104,7 +4130,7 @@
       </c>
       <c r="D43" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   L   [5] = { 4 , 0x7F, 0x40, 0x40, 0x40};</v>
+        <v>static const PROGMEM uint8_t   L   [5] = { 4 , 0x7F, 0x40, 0x40, 0x40};</v>
       </c>
       <c r="E43" s="55" t="s">
         <v>126</v>
@@ -4130,7 +4156,7 @@
       </c>
       <c r="D44" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   M   [8] = { 7 , 0x7F, 0x03, 0x06, 0xC, 0x06, 0x03, 0x7F};</v>
+        <v>static const PROGMEM uint8_t   M   [8] = { 7 , 0x7F, 0x03, 0x06, 0xC, 0x06, 0x03, 0x7F};</v>
       </c>
       <c r="E44" s="55" t="s">
         <v>126</v>
@@ -4156,7 +4182,7 @@
       </c>
       <c r="D45" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   N   [7] = { 6 , 0x7F, 0x03, 0xE, 0x38, 0x60, 0x7F};</v>
+        <v>static const PROGMEM uint8_t   N   [7] = { 6 , 0x7F, 0x03, 0xE, 0x38, 0x60, 0x7F};</v>
       </c>
       <c r="E45" s="55" t="s">
         <v>126</v>
@@ -4182,7 +4208,7 @@
       </c>
       <c r="D46" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   O   [6] = { 5 , 0x3E, 0x41, 0x41, 0x41, 0x3E};</v>
+        <v>static const PROGMEM uint8_t   O   [6] = { 5 , 0x3E, 0x41, 0x41, 0x41, 0x3E};</v>
       </c>
       <c r="E46" s="55" t="s">
         <v>126</v>
@@ -4208,7 +4234,7 @@
       </c>
       <c r="D47" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   P   [5] = { 4 , 0x7F, 0x09, 0x09, 0x06};</v>
+        <v>static const PROGMEM uint8_t   P   [5] = { 4 , 0x7F, 0x09, 0x09, 0x06};</v>
       </c>
       <c r="E47" s="55" t="s">
         <v>126</v>
@@ -4234,7 +4260,7 @@
       </c>
       <c r="D48" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   Q   [7] = { 6 , 0x3E, 0x41, 0x41, 0x51, 0x3E, 0x40};</v>
+        <v>static const PROGMEM uint8_t   Q   [7] = { 6 , 0x3E, 0x41, 0x41, 0x51, 0x3E, 0x40};</v>
       </c>
       <c r="E48" s="55" t="s">
         <v>126</v>
@@ -4260,7 +4286,7 @@
       </c>
       <c r="D49" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   R   [5] = { 4 , 0x7F, 0x09, 0x19, 0x66};</v>
+        <v>static const PROGMEM uint8_t   R   [5] = { 4 , 0x7F, 0x09, 0x19, 0x66};</v>
       </c>
       <c r="E49" s="55" t="s">
         <v>126</v>
@@ -4286,7 +4312,7 @@
       </c>
       <c r="D50" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   S   [5] = { 4 , 0x46, 0x49, 0x49, 0x31};</v>
+        <v>static const PROGMEM uint8_t   S   [5] = { 4 , 0x46, 0x49, 0x49, 0x31};</v>
       </c>
       <c r="E50" s="55" t="s">
         <v>126</v>
@@ -4312,7 +4338,7 @@
       </c>
       <c r="D51" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   T   [6] = { 5 , 0x01, 0x01, 0x7F, 0x01, 0x01};</v>
+        <v>static const PROGMEM uint8_t   T   [6] = { 5 , 0x01, 0x01, 0x7F, 0x01, 0x01};</v>
       </c>
       <c r="E51" s="55" t="s">
         <v>126</v>
@@ -4338,7 +4364,7 @@
       </c>
       <c r="D52" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   U   [6] = { 5 , 0x3F, 0x40, 0x40, 0x40, 0x3F};</v>
+        <v>static const PROGMEM uint8_t   U   [6] = { 5 , 0x3F, 0x40, 0x40, 0x40, 0x3F};</v>
       </c>
       <c r="E52" s="55" t="s">
         <v>126</v>
@@ -4364,7 +4390,7 @@
       </c>
       <c r="D53" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   V   [6] = { 5 , 0x07, 0x18, 0x20, 0x18, 0x07};</v>
+        <v>static const PROGMEM uint8_t   V   [6] = { 5 , 0x07, 0x18, 0x20, 0x18, 0x07};</v>
       </c>
       <c r="E53" s="55" t="s">
         <v>126</v>
@@ -4390,7 +4416,7 @@
       </c>
       <c r="D54" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   W   [8] = { 7 , 0x07, 0x18, 0x20, 0x10, 0x20, 0x18, 0x07};</v>
+        <v>static const PROGMEM uint8_t   W   [8] = { 7 , 0x07, 0x18, 0x20, 0x10, 0x20, 0x18, 0x07};</v>
       </c>
       <c r="E54" s="55" t="s">
         <v>126</v>
@@ -4416,7 +4442,7 @@
       </c>
       <c r="D55" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   X   [6] = { 5 , 0x63, 0x14, 0x08, 0x14, 0x63};</v>
+        <v>static const PROGMEM uint8_t   X   [6] = { 5 , 0x63, 0x14, 0x08, 0x14, 0x63};</v>
       </c>
       <c r="E55" s="55" t="s">
         <v>126</v>
@@ -4442,7 +4468,7 @@
       </c>
       <c r="D56" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   Y   [6] = { 5 , 0x03, 0x04, 0x78, 0x04, 0x03};</v>
+        <v>static const PROGMEM uint8_t   Y   [6] = { 5 , 0x03, 0x04, 0x78, 0x04, 0x03};</v>
       </c>
       <c r="E56" s="55" t="s">
         <v>126</v>
@@ -4468,7 +4494,7 @@
       </c>
       <c r="D57" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   Z   [6] = { 5 , 0x61, 0x51, 0x49, 0x45, 0x43};</v>
+        <v>static const PROGMEM uint8_t   Z   [6] = { 5 , 0x61, 0x51, 0x49, 0x45, 0x43};</v>
       </c>
       <c r="E57" s="55" t="s">
         <v>126</v>
@@ -4509,7 +4535,7 @@
       </c>
       <c r="D59" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   zero   [6] = { 5 , 0x3E, 0x41, 0x49, 0x41, 0x3E};</v>
+        <v>static const PROGMEM uint8_t   zero   [6] = { 5 , 0x3E, 0x41, 0x49, 0x41, 0x3E};</v>
       </c>
       <c r="E59" s="55" t="s">
         <v>97</v>
@@ -4535,7 +4561,7 @@
       </c>
       <c r="D60" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   one   [6] = { 5 , 0x44, 0x42, 0x7F, 0x40, 0x40};</v>
+        <v>static const PROGMEM uint8_t   one   [6] = { 5 , 0x44, 0x42, 0x7F, 0x40, 0x40};</v>
       </c>
       <c r="E60" s="55" t="s">
         <v>97</v>
@@ -4561,7 +4587,7 @@
       </c>
       <c r="D61" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   two   [6] = { 5 , 0x72, 0x51, 0x59, 0x4D, 0x46};</v>
+        <v>static const PROGMEM uint8_t   two   [6] = { 5 , 0x72, 0x51, 0x59, 0x4D, 0x46};</v>
       </c>
       <c r="E61" s="55" t="s">
         <v>97</v>
@@ -4587,7 +4613,7 @@
       </c>
       <c r="D62" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   three   [6] = { 5 , 0x22, 0x41, 0x49, 0x49, 0x36};</v>
+        <v>static const PROGMEM uint8_t   three   [6] = { 5 , 0x22, 0x41, 0x49, 0x49, 0x36};</v>
       </c>
       <c r="E62" s="55" t="s">
         <v>97</v>
@@ -4613,7 +4639,7 @@
       </c>
       <c r="D63" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   four   [6] = { 5 , 0x18, 0x16, 0x11, 0x7F, 0x10};</v>
+        <v>static const PROGMEM uint8_t   four   [6] = { 5 , 0x18, 0x16, 0x11, 0x7F, 0x10};</v>
       </c>
       <c r="E63" s="55" t="s">
         <v>97</v>
@@ -4639,7 +4665,7 @@
       </c>
       <c r="D64" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   five   [6] = { 5 , 0x4F, 0x49, 0x49, 0x49, 0x31};</v>
+        <v>static const PROGMEM uint8_t   five   [6] = { 5 , 0x4F, 0x49, 0x49, 0x49, 0x31};</v>
       </c>
       <c r="E64" s="55" t="s">
         <v>97</v>
@@ -4665,7 +4691,7 @@
       </c>
       <c r="D65" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   six   [6] = { 5 , 0x3E, 0x49, 0x49, 0x49, 0x30};</v>
+        <v>static const PROGMEM uint8_t   six   [6] = { 5 , 0x3E, 0x49, 0x49, 0x49, 0x30};</v>
       </c>
       <c r="E65" s="55" t="s">
         <v>97</v>
@@ -4691,7 +4717,7 @@
       </c>
       <c r="D66" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   seven   [6] = { 5 , 0x61, 0x11, 0x09, 0x05, 0x03};</v>
+        <v>static const PROGMEM uint8_t   seven   [6] = { 5 , 0x61, 0x11, 0x09, 0x05, 0x03};</v>
       </c>
       <c r="E66" s="55" t="s">
         <v>97</v>
@@ -4717,7 +4743,7 @@
       </c>
       <c r="D67" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   eight   [6] = { 5 , 0x36, 0x49, 0x49, 0x49, 0x36};</v>
+        <v>static const PROGMEM uint8_t   eight   [6] = { 5 , 0x36, 0x49, 0x49, 0x49, 0x36};</v>
       </c>
       <c r="E67" s="55" t="s">
         <v>97</v>
@@ -4743,7 +4769,7 @@
       </c>
       <c r="D68" s="61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>static const uint8_t   nine   [6] = { 5 , 0x06, 0x49, 0x49, 0x49, 0x3E};</v>
+        <v>static const PROGMEM uint8_t   nine   [6] = { 5 , 0x06, 0x49, 0x49, 0x49, 0x3E};</v>
       </c>
       <c r="E68" s="55" t="s">
         <v>97</v>
@@ -4778,9 +4804,8 @@
       <c r="B70" s="50"/>
       <c r="C70" s="50"/>
       <c r="D70" s="61" t="str">
-        <f t="shared" ref="D70:D133" ca="1" si="3">IF(ISBLANK(E70)," ",
-"static const uint8_t   " &amp; (INDIRECT("'"&amp;E70&amp;"'!W"&amp;(VALUE(F70)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E70&amp;"'!X"&amp;(VALUE(F70)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E70&amp;"'!X"&amp;(VALUE(F70)+4))&amp;" , "&amp;INDIRECT("'"&amp;E70&amp;"'!Y"&amp;(VALUE(F70)+4))&amp;"};")</f>
-        <v>static const uint8_t   exclamation   [2] = { 1 , 0x9F};</v>
+        <f t="shared" ref="D70:D133" ca="1" si="3">IF(ISBLANK(E70)," ","static const PROGMEM uint8_t   " &amp; (INDIRECT("'"&amp;E70&amp;"'!W"&amp;(VALUE(F70)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E70&amp;"'!X"&amp;(VALUE(F70)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E70&amp;"'!X"&amp;(VALUE(F70)+4))&amp;" , "&amp;INDIRECT("'"&amp;E70&amp;"'!Y"&amp;(VALUE(F70)+4))&amp;"};")</f>
+        <v>static const PROGMEM uint8_t   exclamation   [2] = { 1 , 0x9F};</v>
       </c>
       <c r="E70" s="55" t="s">
         <v>125</v>
@@ -4801,7 +4826,7 @@
       <c r="C71" s="50"/>
       <c r="D71" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   quote   [4] = { 3 , 0x07, 0x00, 0x07};</v>
+        <v>static const PROGMEM uint8_t   quote   [4] = { 3 , 0x07, 0x00, 0x07};</v>
       </c>
       <c r="E71" s="55" t="s">
         <v>125</v>
@@ -4822,7 +4847,7 @@
       <c r="C72" s="50"/>
       <c r="D72" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   hash   [6] = { 5 , 0x14, 0x7F, 0x14, 0x7F, 0x14};</v>
+        <v>static const PROGMEM uint8_t   hash   [6] = { 5 , 0x14, 0x7F, 0x14, 0x7F, 0x14};</v>
       </c>
       <c r="E72" s="55" t="s">
         <v>125</v>
@@ -4843,7 +4868,7 @@
       <c r="C73" s="50"/>
       <c r="D73" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   dollar   [6] = { 5 , 0x48, 0x54, 0xFE, 0x54, 0x24};</v>
+        <v>static const PROGMEM uint8_t   dollar   [6] = { 5 , 0x48, 0x54, 0xFE, 0x54, 0x24};</v>
       </c>
       <c r="E73" s="55" t="s">
         <v>125</v>
@@ -4864,7 +4889,7 @@
       <c r="C74" s="50"/>
       <c r="D74" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   percent   [6] = { 5 , 0x66, 0x36, 0x18, 0x6C, 0x66};</v>
+        <v>static const PROGMEM uint8_t   percent   [6] = { 5 , 0x66, 0x36, 0x18, 0x6C, 0x66};</v>
       </c>
       <c r="E74" s="55" t="s">
         <v>125</v>
@@ -4885,7 +4910,7 @@
       <c r="C75" s="50"/>
       <c r="D75" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   ampersand   [7] = { 6 , 0x34, 0x4A, 0x4A, 0x54, 0x20, 0x40};</v>
+        <v>static const PROGMEM uint8_t   ampersand   [7] = { 6 , 0x34, 0x4A, 0x4A, 0x54, 0x20, 0x40};</v>
       </c>
       <c r="E75" s="55" t="s">
         <v>125</v>
@@ -4906,7 +4931,7 @@
       <c r="C76" s="50"/>
       <c r="D76" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   apostrophe   [2] = { 1 , 0x07};</v>
+        <v>static const PROGMEM uint8_t   apostrophe   [2] = { 1 , 0x07};</v>
       </c>
       <c r="E76" s="55" t="s">
         <v>125</v>
@@ -4927,7 +4952,7 @@
       <c r="C77" s="50"/>
       <c r="D77" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   openParenthesis   [4] = { 3 , 0x1C, 0x22, 0x41};</v>
+        <v>static const PROGMEM uint8_t   openParenthesis   [4] = { 3 , 0x1C, 0x22, 0x41};</v>
       </c>
       <c r="E77" s="55" t="s">
         <v>125</v>
@@ -4948,7 +4973,7 @@
       <c r="C78" s="50"/>
       <c r="D78" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   closeParenthesis   [4] = { 3 , 0x41, 0x22, 0x1C};</v>
+        <v>static const PROGMEM uint8_t   closeParenthesis   [4] = { 3 , 0x41, 0x22, 0x1C};</v>
       </c>
       <c r="E78" s="55" t="s">
         <v>125</v>
@@ -4969,7 +4994,7 @@
       <c r="C79" s="50"/>
       <c r="D79" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   asterix   [3] = { 2 , 0x18, 0x18};</v>
+        <v>static const PROGMEM uint8_t   asterix   [3] = { 2 , 0x18, 0x18};</v>
       </c>
       <c r="E79" s="55" t="s">
         <v>125</v>
@@ -4990,7 +5015,7 @@
       <c r="C80" s="50"/>
       <c r="D80" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   plus   [6] = { 5 , 0x10, 0x10, 0x7C, 0x10, 0x10};</v>
+        <v>static const PROGMEM uint8_t   plus   [6] = { 5 , 0x10, 0x10, 0x7C, 0x10, 0x10};</v>
       </c>
       <c r="E80" s="55" t="s">
         <v>125</v>
@@ -5011,7 +5036,7 @@
       <c r="C81" s="50"/>
       <c r="D81" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   comma   [3] = { 2 , 0xC0, 0x60};</v>
+        <v>static const PROGMEM uint8_t   comma   [3] = { 2 , 0xC0, 0x60};</v>
       </c>
       <c r="E81" s="55" t="s">
         <v>125</v>
@@ -5036,7 +5061,7 @@
       <c r="C82" s="50"/>
       <c r="D82" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   dash   [6] = { 5 , 0x10, 0x10, 0x10, 0x10, 0x10};</v>
+        <v>static const PROGMEM uint8_t   dash   [6] = { 5 , 0x10, 0x10, 0x10, 0x10, 0x10};</v>
       </c>
       <c r="E82" s="55" t="s">
         <v>125</v>
@@ -5061,7 +5086,7 @@
       <c r="C83" s="50"/>
       <c r="D83" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   dot   [3] = { 2 , 0x60, 0x60};</v>
+        <v>static const PROGMEM uint8_t   dot   [3] = { 2 , 0x60, 0x60};</v>
       </c>
       <c r="E83" s="55" t="s">
         <v>125</v>
@@ -5086,7 +5111,7 @@
       <c r="C84" s="50"/>
       <c r="D84" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   slash   [4] = { 3 , 0x70, 0x1C, 0x07};</v>
+        <v>static const PROGMEM uint8_t   slash   [4] = { 3 , 0x70, 0x1C, 0x07};</v>
       </c>
       <c r="E84" s="55" t="s">
         <v>125</v>
@@ -5111,7 +5136,7 @@
       <c r="C85" s="50"/>
       <c r="D85" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   colon   [3] = { 2 , 0x6C, 0x6C};</v>
+        <v>static const PROGMEM uint8_t   colon   [3] = { 2 , 0x6C, 0x6C};</v>
       </c>
       <c r="E85" s="55" t="s">
         <v>125</v>
@@ -5136,7 +5161,7 @@
       <c r="C86" s="50"/>
       <c r="D86" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   semicolon   [3] = { 2 , 0xCC, 0x6C};</v>
+        <v>static const PROGMEM uint8_t   semicolon   [3] = { 2 , 0xCC, 0x6C};</v>
       </c>
       <c r="E86" s="55" t="s">
         <v>125</v>
@@ -5157,7 +5182,7 @@
       <c r="C87" s="50"/>
       <c r="D87" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   lessThan   [5] = { 4 , 0x10, 0x38, 0x6C, 0x44};</v>
+        <v>static const PROGMEM uint8_t   lessThan   [5] = { 4 , 0x10, 0x38, 0x6C, 0x44};</v>
       </c>
       <c r="E87" s="55" t="s">
         <v>125</v>
@@ -5178,7 +5203,7 @@
       <c r="C88" s="50"/>
       <c r="D88" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   equals   [6] = { 5 , 0x28, 0x28, 0x28, 0x28, 0x28};</v>
+        <v>static const PROGMEM uint8_t   equals   [6] = { 5 , 0x28, 0x28, 0x28, 0x28, 0x28};</v>
       </c>
       <c r="E88" s="55" t="s">
         <v>125</v>
@@ -5199,7 +5224,7 @@
       <c r="C89" s="50"/>
       <c r="D89" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   greatherThan   [5] = { 4 , 0x44, 0x6C, 0x38, 0x10};</v>
+        <v>static const PROGMEM uint8_t   greatherThan   [5] = { 4 , 0x44, 0x6C, 0x38, 0x10};</v>
       </c>
       <c r="E89" s="55" t="s">
         <v>125</v>
@@ -5220,7 +5245,7 @@
       <c r="C90" s="50"/>
       <c r="D90" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   question   [5] = { 4 , 0x02, 0x51, 0x09, 0x06};</v>
+        <v>static const PROGMEM uint8_t   question   [5] = { 4 , 0x02, 0x51, 0x09, 0x06};</v>
       </c>
       <c r="E90" s="55" t="s">
         <v>125</v>
@@ -5241,7 +5266,7 @@
       <c r="C91" s="50"/>
       <c r="D91" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   at   [7] = { 6 , 0x3C, 0x42, 0x5A, 0x5A, 0x52, 0x1C};</v>
+        <v>static const PROGMEM uint8_t   at   [7] = { 6 , 0x3C, 0x42, 0x5A, 0x5A, 0x52, 0x1C};</v>
       </c>
       <c r="E91" s="55" t="s">
         <v>125</v>
@@ -5266,7 +5291,7 @@
       <c r="C92" s="50"/>
       <c r="D92" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   openBracket   [3] = { 2 , 0x7F, 0x41};</v>
+        <v>static const PROGMEM uint8_t   openBracket   [3] = { 2 , 0x7F, 0x41};</v>
       </c>
       <c r="E92" s="55" t="s">
         <v>125</v>
@@ -5291,7 +5316,7 @@
       <c r="C93" s="50"/>
       <c r="D93" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   closeBracket   [3] = { 2 , 0x41, 0x7F};</v>
+        <v>static const PROGMEM uint8_t   closeBracket   [3] = { 2 , 0x41, 0x7F};</v>
       </c>
       <c r="E93" s="55" t="s">
         <v>125</v>
@@ -5316,7 +5341,7 @@
       <c r="C94" s="50"/>
       <c r="D94" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   openBrace   [4] = { 3 , 0x08, 0x36, 0x41};</v>
+        <v>static const PROGMEM uint8_t   openBrace   [4] = { 3 , 0x08, 0x36, 0x41};</v>
       </c>
       <c r="E94" s="55" t="s">
         <v>125</v>
@@ -5341,7 +5366,7 @@
       <c r="C95" s="50"/>
       <c r="D95" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   closeBrace   [4] = { 3 , 0x41, 0x36, 0x08};</v>
+        <v>static const PROGMEM uint8_t   closeBrace   [4] = { 3 , 0x41, 0x36, 0x08};</v>
       </c>
       <c r="E95" s="55" t="s">
         <v>125</v>
@@ -5366,7 +5391,7 @@
       <c r="C96" s="50"/>
       <c r="D96" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   backslash   [4] = { 3 , 0x07, 0x1C, 0x70};</v>
+        <v>static const PROGMEM uint8_t   backslash   [4] = { 3 , 0x07, 0x1C, 0x70};</v>
       </c>
       <c r="E96" s="55" t="s">
         <v>125</v>
@@ -5391,7 +5416,7 @@
       <c r="C97" s="50"/>
       <c r="D97" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   hat   [6] = { 5 , 0x04, 0x02, 0x01, 0x02, 0x04};</v>
+        <v>static const PROGMEM uint8_t   hat   [6] = { 5 , 0x04, 0x02, 0x01, 0x02, 0x04};</v>
       </c>
       <c r="E97" s="55" t="s">
         <v>125</v>
@@ -5416,7 +5441,7 @@
       <c r="C98" s="50"/>
       <c r="D98" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   underscore   [6] = { 5 , 0x40, 0x40, 0x40, 0x40, 0x40};</v>
+        <v>static const PROGMEM uint8_t   underscore   [6] = { 5 , 0x40, 0x40, 0x40, 0x40, 0x40};</v>
       </c>
       <c r="E98" s="55" t="s">
         <v>125</v>
@@ -5441,7 +5466,7 @@
       <c r="C99" s="50"/>
       <c r="D99" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   accent   [3] = { 2 , 0x01, 0x02};</v>
+        <v>static const PROGMEM uint8_t   accent   [3] = { 2 , 0x01, 0x02};</v>
       </c>
       <c r="E99" s="55" t="s">
         <v>125</v>
@@ -5466,7 +5491,7 @@
       <c r="C100" s="50"/>
       <c r="D100" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   bar   [2] = { 1 , 0xFF};</v>
+        <v>static const PROGMEM uint8_t   bar   [2] = { 1 , 0xFF};</v>
       </c>
       <c r="E100" s="55" t="s">
         <v>125</v>
@@ -5491,7 +5516,7 @@
       <c r="C101" s="50"/>
       <c r="D101" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   tilde   [6] = { 5 , 0x10, 0x08, 0x10, 0x20, 0x10};</v>
+        <v>static const PROGMEM uint8_t   tilde   [6] = { 5 , 0x10, 0x08, 0x10, 0x20, 0x10};</v>
       </c>
       <c r="E101" s="55" t="s">
         <v>125</v>
@@ -5535,7 +5560,7 @@
       <c r="C103" s="50"/>
       <c r="D103" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   accentedA   [5] = { 4 , 0x20, 0x55, 0x55, 0x39};</v>
+        <v>static const PROGMEM uint8_t   accentedA   [5] = { 4 , 0x20, 0x55, 0x55, 0x39};</v>
       </c>
       <c r="E103" s="55" t="s">
         <v>124</v>
@@ -5560,7 +5585,7 @@
       <c r="C104" s="50"/>
       <c r="D104" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   accentedE   [5] = { 4 , 0x38, 0x55, 0x55, 0x09};</v>
+        <v>static const PROGMEM uint8_t   accentedE   [5] = { 4 , 0x38, 0x55, 0x55, 0x09};</v>
       </c>
       <c r="E104" s="55" t="s">
         <v>124</v>
@@ -5585,7 +5610,7 @@
       <c r="C105" s="50"/>
       <c r="D105" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   accentedO   [6] = { 5 , 0x38, 0x45, 0x45, 0x45, 0x38};</v>
+        <v>static const PROGMEM uint8_t   accentedO   [6] = { 5 , 0x38, 0x45, 0x45, 0x45, 0x38};</v>
       </c>
       <c r="E105" s="55" t="s">
         <v>124</v>
@@ -5610,7 +5635,7 @@
       <c r="C106" s="50"/>
       <c r="D106" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   accentedI   [4] = { 3 , 0x00, 0x7D, 0x01};</v>
+        <v>static const PROGMEM uint8_t   accentedI   [4] = { 3 , 0x00, 0x7D, 0x01};</v>
       </c>
       <c r="E106" s="55" t="s">
         <v>124</v>
@@ -5635,7 +5660,7 @@
       <c r="C107" s="50"/>
       <c r="D107" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   accentedU   [6] = { 5 , 0x00, 0x3C, 0x41, 0x41, 0x7D};</v>
+        <v>static const PROGMEM uint8_t   accentedU   [6] = { 5 , 0x00, 0x3C, 0x41, 0x41, 0x7D};</v>
       </c>
       <c r="E107" s="55" t="s">
         <v>124</v>
@@ -5660,7 +5685,7 @@
       <c r="C108" s="50"/>
       <c r="D108" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   degree   [5] = { 4 , 0x06, 0x09, 0x09, 0x06};</v>
+        <v>static const PROGMEM uint8_t   degree   [5] = { 4 , 0x06, 0x09, 0x09, 0x06};</v>
       </c>
       <c r="E108" s="55" t="s">
         <v>124</v>
@@ -5685,7 +5710,7 @@
       <c r="C109" s="50"/>
       <c r="D109" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowUp   [8] = { 7 , 0x08, 0x04, 0x02, 0xFF, 0x02, 0x04, 0x08};</v>
+        <v>static const PROGMEM uint8_t   arrowUp   [8] = { 7 , 0x08, 0x04, 0x02, 0xFF, 0x02, 0x04, 0x08};</v>
       </c>
       <c r="E109" s="55" t="s">
         <v>124</v>
@@ -5710,7 +5735,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowDown   [8] = { 7 , 0x10, 0x20, 0x40, 0xFF, 0x40, 0x20, 0x10};</v>
+        <v>static const PROGMEM uint8_t   arrowDown   [8] = { 7 , 0x10, 0x20, 0x40, 0xFF, 0x40, 0x20, 0x10};</v>
       </c>
       <c r="E110" s="55" t="s">
         <v>124</v>
@@ -5735,7 +5760,7 @@
       <c r="C111" s="50"/>
       <c r="D111" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowLeft   [9] = { 8 , 0x10, 0x38, 0x54, 0x92, 0x10, 0x10, 0x10, 0x10};</v>
+        <v>static const PROGMEM uint8_t   arrowLeft   [9] = { 8 , 0x10, 0x38, 0x54, 0x92, 0x10, 0x10, 0x10, 0x10};</v>
       </c>
       <c r="E111" s="55" t="s">
         <v>124</v>
@@ -5760,7 +5785,7 @@
       <c r="C112" s="50"/>
       <c r="D112" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowRight   [9] = { 8 , 0x10, 0x10, 0x10, 0x10, 0x92, 0x54, 0x38, 0x10};</v>
+        <v>static const PROGMEM uint8_t   arrowRight   [9] = { 8 , 0x10, 0x10, 0x10, 0x10, 0x92, 0x54, 0x38, 0x10};</v>
       </c>
       <c r="E112" s="55" t="s">
         <v>124</v>
@@ -5785,7 +5810,7 @@
       <c r="C113" s="50"/>
       <c r="D113" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowUpRight   [9] = { 8 , 0x80, 0x40, 0x20, 0x11, 0x09, 0x05, 0x03, 0x1F};</v>
+        <v>static const PROGMEM uint8_t   arrowUpRight   [9] = { 8 , 0x80, 0x40, 0x20, 0x11, 0x09, 0x05, 0x03, 0x1F};</v>
       </c>
       <c r="E113" s="55" t="s">
         <v>124</v>
@@ -5810,7 +5835,7 @@
       <c r="C114" s="50"/>
       <c r="D114" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowDownRight   [9] = { 8 , 0x01, 0x02, 0x04, 0x88, 0x90, 0xA0, 0xC0, 0xF8};</v>
+        <v>static const PROGMEM uint8_t   arrowDownRight   [9] = { 8 , 0x01, 0x02, 0x04, 0x88, 0x90, 0xA0, 0xC0, 0xF8};</v>
       </c>
       <c r="E114" s="55" t="s">
         <v>124</v>
@@ -5835,7 +5860,7 @@
       <c r="C115" s="50"/>
       <c r="D115" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowDownLeft   [9] = { 8 , 0xF8, 0xC0, 0xA0, 0x90, 0x88, 0x04, 0x02, 0x01};</v>
+        <v>static const PROGMEM uint8_t   arrowDownLeft   [9] = { 8 , 0xF8, 0xC0, 0xA0, 0x90, 0x88, 0x04, 0x02, 0x01};</v>
       </c>
       <c r="E115" s="55" t="s">
         <v>124</v>
@@ -5860,7 +5885,7 @@
       <c r="C116" s="50"/>
       <c r="D116" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   arrowUpLeft   [9] = { 8 , 0x1F, 0x03, 0x05, 0x09, 0x11, 0x20, 0x40, 0x80};</v>
+        <v>static const PROGMEM uint8_t   arrowUpLeft   [9] = { 8 , 0x1F, 0x03, 0x05, 0x09, 0x11, 0x20, 0x40, 0x80};</v>
       </c>
       <c r="E116" s="55" t="s">
         <v>124</v>
@@ -5885,7 +5910,7 @@
       <c r="C117" s="50"/>
       <c r="D117" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   copyright   [7] = { 6 , 0x7C, 0x82, 0xBA, 0xAA, 0x82, 0x7C};</v>
+        <v>static const PROGMEM uint8_t   copyright   [7] = { 6 , 0x7C, 0x82, 0xBA, 0xAA, 0x82, 0x7C};</v>
       </c>
       <c r="E117" s="55" t="s">
         <v>124</v>
@@ -5910,7 +5935,7 @@
       <c r="C118" s="50"/>
       <c r="D118" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   unknown   [4] = { 3 , 0x3E, 0x3E, 0x3E};</v>
+        <v>static const PROGMEM uint8_t   unknown   [4] = { 3 , 0x3E, 0x3E, 0x3E};</v>
       </c>
       <c r="E118" s="55" t="s">
         <v>124</v>
@@ -5935,7 +5960,7 @@
       <c r="C119" s="50"/>
       <c r="D119" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expZero   [4] = { 3 , 0xE, 0x11, 0xE};</v>
+        <v>static const PROGMEM uint8_t   expZero   [4] = { 3 , 0xE, 0x11, 0xE};</v>
       </c>
       <c r="E119" s="55" t="s">
         <v>124</v>
@@ -5959,7 +5984,7 @@
       <c r="B120" s="50"/>
       <c r="D120" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expOne   [4] = { 3 , 0x02, 0x01, 0x1F};</v>
+        <v>static const PROGMEM uint8_t   expOne   [4] = { 3 , 0x02, 0x01, 0x1F};</v>
       </c>
       <c r="E120" s="55" t="s">
         <v>124</v>
@@ -5983,7 +6008,7 @@
       <c r="B121" s="50"/>
       <c r="D121" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expTwo   [4] = { 3 , 0x19, 0x15, 0x12};</v>
+        <v>static const PROGMEM uint8_t   expTwo   [4] = { 3 , 0x19, 0x15, 0x12};</v>
       </c>
       <c r="E121" s="55" t="s">
         <v>124</v>
@@ -6007,7 +6032,7 @@
       <c r="B122" s="50"/>
       <c r="D122" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expThree   [4] = { 3 , 0x11, 0x15, 0xA};</v>
+        <v>static const PROGMEM uint8_t   expThree   [4] = { 3 , 0x11, 0x15, 0xA};</v>
       </c>
       <c r="E122" s="55" t="s">
         <v>124</v>
@@ -6031,7 +6056,7 @@
       <c r="B123" s="50"/>
       <c r="D123" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expFour   [4] = { 3 , 0xC, 0xA, 0x1D};</v>
+        <v>static const PROGMEM uint8_t   expFour   [4] = { 3 , 0xC, 0xA, 0x1D};</v>
       </c>
       <c r="E123" s="55" t="s">
         <v>124</v>
@@ -6055,7 +6080,7 @@
       <c r="B124" s="50"/>
       <c r="D124" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expFive   [4] = { 3 , 0x17, 0x15, 0x09};</v>
+        <v>static const PROGMEM uint8_t   expFive   [4] = { 3 , 0x17, 0x15, 0x09};</v>
       </c>
       <c r="E124" s="55" t="s">
         <v>124</v>
@@ -6079,7 +6104,7 @@
       <c r="B125" s="50"/>
       <c r="D125" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expSix   [4] = { 3 , 0x1E, 0x15, 0x1D};</v>
+        <v>static const PROGMEM uint8_t   expSix   [4] = { 3 , 0x1E, 0x15, 0x1D};</v>
       </c>
       <c r="E125" s="55" t="s">
         <v>124</v>
@@ -6103,7 +6128,7 @@
       <c r="B126" s="50"/>
       <c r="D126" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expSeven   [4] = { 3 , 0x19, 0x05, 0x03};</v>
+        <v>static const PROGMEM uint8_t   expSeven   [4] = { 3 , 0x19, 0x05, 0x03};</v>
       </c>
       <c r="E126" s="55" t="s">
         <v>124</v>
@@ -6127,7 +6152,7 @@
       <c r="B127" s="50"/>
       <c r="D127" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expEight   [4] = { 3 , 0x1B, 0x15, 0x1B};</v>
+        <v>static const PROGMEM uint8_t   expEight   [4] = { 3 , 0x1B, 0x15, 0x1B};</v>
       </c>
       <c r="E127" s="55" t="s">
         <v>124</v>
@@ -6151,7 +6176,7 @@
       <c r="B128" s="50"/>
       <c r="D128" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   expNine   [4] = { 3 , 0x17, 0x15, 0xF};</v>
+        <v>static const PROGMEM uint8_t   expNine   [4] = { 3 , 0x17, 0x15, 0xF};</v>
       </c>
       <c r="E128" s="55" t="s">
         <v>124</v>
@@ -6175,7 +6200,7 @@
       <c r="B129" s="50"/>
       <c r="D129" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E129" s="55" t="s">
         <v>124</v>
@@ -6199,7 +6224,7 @@
       <c r="B130" s="50"/>
       <c r="D130" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E130" s="55" t="s">
         <v>124</v>
@@ -6223,7 +6248,7 @@
       <c r="B131" s="50"/>
       <c r="D131" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E131" s="55" t="s">
         <v>124</v>
@@ -6247,7 +6272,7 @@
       <c r="B132" s="50"/>
       <c r="D132" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E132" s="55" t="s">
         <v>124</v>
@@ -6271,7 +6296,7 @@
       <c r="B133" s="50"/>
       <c r="D133" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E133" s="55" t="s">
         <v>124</v>
@@ -6294,9 +6319,8 @@
     <row r="134" spans="2:124">
       <c r="B134" s="50"/>
       <c r="D134" s="61" t="str">
-        <f t="shared" ref="D134:D148" ca="1" si="4">IF(ISBLANK(E134)," ",
-"static const uint8_t   " &amp; (INDIRECT("'"&amp;E134&amp;"'!W"&amp;(VALUE(F134)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E134&amp;"'!X"&amp;(VALUE(F134)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E134&amp;"'!X"&amp;(VALUE(F134)+4))&amp;" , "&amp;INDIRECT("'"&amp;E134&amp;"'!Y"&amp;(VALUE(F134)+4))&amp;"};")</f>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <f t="shared" ref="D134:D148" ca="1" si="4">IF(ISBLANK(E134)," ","static const PROGMEM uint8_t   " &amp; (INDIRECT("'"&amp;E134&amp;"'!W"&amp;(VALUE(F134)+4)))&amp;"   ["&amp;(INDIRECT("'"&amp;E134&amp;"'!X"&amp;(VALUE(F134)+4)) + 1)&amp;   "] = { "&amp;INDIRECT("'"&amp;E134&amp;"'!X"&amp;(VALUE(F134)+4))&amp;" , "&amp;INDIRECT("'"&amp;E134&amp;"'!Y"&amp;(VALUE(F134)+4))&amp;"};")</f>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E134" s="55" t="s">
         <v>124</v>
@@ -6320,7 +6344,7 @@
       <c r="B135" s="50"/>
       <c r="D135" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E135" s="55" t="s">
         <v>124</v>
@@ -6344,7 +6368,7 @@
       <c r="B136" s="50"/>
       <c r="D136" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E136" s="55" t="s">
         <v>124</v>
@@ -6368,7 +6392,7 @@
       <c r="B137" s="50"/>
       <c r="D137" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t   0   [1] = { 0 , 0};</v>
+        <v>static const PROGMEM uint8_t   0   [1] = { 0 , 0};</v>
       </c>
       <c r="E137" s="55" t="s">
         <v>124</v>
@@ -6392,7 +6416,7 @@
       <c r="B138" s="50"/>
       <c r="D138" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E138" s="55" t="s">
         <v>124</v>
@@ -6416,7 +6440,7 @@
       <c r="B139" s="50"/>
       <c r="D139" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E139" s="55" t="s">
         <v>124</v>
@@ -6440,7 +6464,7 @@
       <c r="B140" s="50"/>
       <c r="D140" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E140" s="55" t="s">
         <v>124</v>
@@ -6464,7 +6488,7 @@
       <c r="B141" s="50"/>
       <c r="D141" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E141" s="55" t="s">
         <v>124</v>
@@ -6488,7 +6512,7 @@
       <c r="B142" s="50"/>
       <c r="D142" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E142" s="55" t="s">
         <v>124</v>
@@ -6512,7 +6536,7 @@
       <c r="B143" s="50"/>
       <c r="D143" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E143" s="55" t="s">
         <v>124</v>
@@ -6536,7 +6560,7 @@
       <c r="B144" s="50"/>
       <c r="D144" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E144" s="55" t="s">
         <v>124</v>
@@ -6560,7 +6584,7 @@
       <c r="B145" s="50"/>
       <c r="D145" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E145" s="55" t="s">
         <v>124</v>
@@ -6584,7 +6608,7 @@
       <c r="B146" s="50"/>
       <c r="D146" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E146" s="55" t="s">
         <v>124</v>
@@ -6608,7 +6632,7 @@
       <c r="B147" s="50"/>
       <c r="D147" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E147" s="55" t="s">
         <v>124</v>
@@ -6632,7 +6656,7 @@
       <c r="B148" s="50"/>
       <c r="D148" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>static const uint8_t      [1] = {  , };</v>
+        <v>static const PROGMEM uint8_t      [1] = {  , };</v>
       </c>
       <c r="E148" s="55" t="s">
         <v>124</v>
@@ -8338,8 +8362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="G153" sqref="G153"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8449,7 +8473,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="10">
         <f>IF(ISBLANK(C4),0,1)*1+IF(ISBLANK(C5),0,1)*2+IF(ISBLANK(C6),0,1)*4+IF(ISBLANK(C7),0,1)*8+IF(ISBLANK(C8),0,1)*16+IF(ISBLANK(C9),0,1)*32+IF(ISBLANK(C10),0,1)*64+IF(ISBLANK(C11),0,1)*128</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L4" s="10">
         <f t="shared" ref="L4:R4" si="0">IF(ISBLANK(D4),0,1)*1+IF(ISBLANK(D5),0,1)*2+IF(ISBLANK(D6),0,1)*4+IF(ISBLANK(D7),0,1)*8+IF(ISBLANK(D8),0,1)*16+IF(ISBLANK(D9),0,1)*32+IF(ISBLANK(D10),0,1)*64+IF(ISBLANK(D11),0,1)*128</f>
@@ -8461,11 +8485,11 @@
       </c>
       <c r="N4" s="10">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="O4" s="10">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="P4" s="10">
         <f t="shared" si="0"/>
@@ -8481,11 +8505,11 @@
       </c>
       <c r="S4" s="73">
         <f xml:space="preserve">   IF(VALUE(R4)+VALUE(Q4)+VALUE(P4)+VALUE(O4)+VALUE(N4)+VALUE(M4)+VALUE(L4)+VALUE(K4)=0, 0,   IF(VALUE(R4)+VALUE(Q4)+VALUE(P4)+VALUE(O4)+VALUE(N4)+VALUE(M4)+VALUE(L4)= 0, 1,   IF(VALUE(R4)+VALUE(Q4)+VALUE(P4)+VALUE(O4)+VALUE(N4)+VALUE(M4)= 0, 2,   IF(VALUE(R4)+VALUE(Q4)+VALUE(P4)+VALUE(O4)+VALUE(N4)= 0, 3,   IF(VALUE(R4)+VALUE(Q4)+VALUE(P4)+VALUE(O4)= 0, 4,   IF(VALUE(R4)+VALUE(Q4)+VALUE(P4)= 0, 5,   IF(VALUE(R4)+VALUE(Q4)= 0, 6,   IF(VALUE(R4)= 0, 7,   8))))))))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T4" s="67" t="str">
         <f xml:space="preserve"> IF(S4 &gt; 0, "0x"&amp; TEXT(DEC2HEX(K4), "00")  &amp; IF(S4 &gt; 1, ", " &amp; "0x"&amp; TEXT(DEC2HEX(L4), "00") &amp; IF(S4 &gt; 2, ", " &amp; "0x"&amp; TEXT(DEC2HEX(M4), "00") &amp; IF(S4 &gt; 3, ", " &amp; "0x"&amp; TEXT(DEC2HEX(N4), "00") &amp; IF(S4 &gt; 4, ", " &amp; "0x"&amp; TEXT(DEC2HEX(O4), "00") &amp; IF(S4 &gt; 5, ", " &amp; "0x"&amp; TEXT(DEC2HEX(P4), "00") &amp; IF(S4 &gt; 6, ", " &amp; "0x"&amp; TEXT(DEC2HEX(Q4), "00") &amp; IF(S4 &gt; 7, ", " &amp; "0x"&amp; TEXT(DEC2HEX(R4), "00"),),),),),),),),)</f>
-        <v>0x20, 0x54, 0x54, 0x54, 0x38</v>
+        <v>0x24, 0x54, 0x54, 0x78</v>
       </c>
       <c r="U4" s="13"/>
       <c r="V4" s="24">
@@ -8497,11 +8521,11 @@
       </c>
       <c r="X4" s="19">
         <f t="shared" ref="X4:X29" ca="1" si="2">OFFSET(S$4, V4*8, 0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y4" s="41" t="str">
         <f t="shared" ref="Y4:Y29" ca="1" si="3" xml:space="preserve"> OFFSET(T$4,V4*8,0)</f>
-        <v>0x20, 0x54, 0x54, 0x54, 0x38</v>
+        <v>0x24, 0x54, 0x54, 0x78</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -8545,16 +8569,16 @@
     <row r="6" spans="1:25">
       <c r="A6" s="12"/>
       <c r="B6" s="72"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -8592,10 +8616,10 @@
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="4"/>
@@ -8623,7 +8647,7 @@
       </c>
       <c r="Y7" s="41" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0x30, 0x48, 0x48, 0x7E</v>
+        <v>0x38, 0x44, 0x44, 0x7E</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -8639,9 +8663,7 @@
       <c r="F8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
@@ -8680,10 +8702,10 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="4"/>
@@ -9307,7 +9329,7 @@
       </c>
       <c r="Y22" s="41" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>0x5C, 0x54, 0x74</v>
+        <v>0x58, 0x54, 0x34</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -9527,15 +9549,15 @@
       <c r="J28" s="7"/>
       <c r="K28" s="10">
         <f t="shared" ref="K28:R28" si="8">IF(ISBLANK(C28),0,1)*1+IF(ISBLANK(C29),0,1)*2+IF(ISBLANK(C30),0,1)*4+IF(ISBLANK(C31),0,1)*8+IF(ISBLANK(C32),0,1)*16+IF(ISBLANK(C33),0,1)*32+IF(ISBLANK(C34),0,1)*64+IF(ISBLANK(C35),0,1)*128</f>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L28" s="10">
         <f t="shared" si="8"/>
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M28" s="10">
         <f t="shared" si="8"/>
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="N28" s="10">
         <f t="shared" si="8"/>
@@ -9563,7 +9585,7 @@
       </c>
       <c r="T28" s="67" t="str">
         <f t="shared" ref="T28" si="9" xml:space="preserve"> IF(S28 &gt; 0, "0x"&amp; TEXT(DEC2HEX(K28), "00")  &amp; IF(S28 &gt; 1, ", " &amp; "0x"&amp; TEXT(DEC2HEX(L28), "00") &amp; IF(S28 &gt; 2, ", " &amp; "0x"&amp; TEXT(DEC2HEX(M28), "00") &amp; IF(S28 &gt; 3, ", " &amp; "0x"&amp; TEXT(DEC2HEX(N28), "00") &amp; IF(S28 &gt; 4, ", " &amp; "0x"&amp; TEXT(DEC2HEX(O28), "00") &amp; IF(S28 &gt; 5, ", " &amp; "0x"&amp; TEXT(DEC2HEX(P28), "00") &amp; IF(S28 &gt; 6, ", " &amp; "0x"&amp; TEXT(DEC2HEX(Q28), "00") &amp; IF(S28 &gt; 7, ", " &amp; "0x"&amp; TEXT(DEC2HEX(R28), "00"),),),),),),),),)</f>
-        <v>0x30, 0x48, 0x48, 0x7E</v>
+        <v>0x38, 0x44, 0x44, 0x7E</v>
       </c>
       <c r="U28" s="12"/>
       <c r="V28" s="24">
@@ -9626,8 +9648,12 @@
       <c r="A30" s="12"/>
       <c r="B30" s="72"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="F30" s="5" t="s">
         <v>35</v>
       </c>
@@ -9654,13 +9680,11 @@
     <row r="31" spans="1:25">
       <c r="A31" s="12"/>
       <c r="B31" s="72"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="C31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
         <v>35</v>
       </c>
@@ -13581,7 +13605,7 @@
       <c r="J148" s="7"/>
       <c r="K148" s="10">
         <f t="shared" ref="K148:R148" si="38">IF(ISBLANK(C148),0,1)*1+IF(ISBLANK(C149),0,1)*2+IF(ISBLANK(C150),0,1)*4+IF(ISBLANK(C151),0,1)*8+IF(ISBLANK(C152),0,1)*16+IF(ISBLANK(C153),0,1)*32+IF(ISBLANK(C154),0,1)*64+IF(ISBLANK(C155),0,1)*128</f>
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L148" s="10">
         <f t="shared" si="38"/>
@@ -13589,7 +13613,7 @@
       </c>
       <c r="M148" s="10">
         <f t="shared" si="38"/>
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="N148" s="10">
         <f t="shared" si="38"/>
@@ -13617,7 +13641,7 @@
       </c>
       <c r="T148" s="67" t="str">
         <f t="shared" ref="T148" si="39" xml:space="preserve"> IF(S148 &gt; 0, "0x"&amp; TEXT(DEC2HEX(K148), "00")  &amp; IF(S148 &gt; 1, ", " &amp; "0x"&amp; TEXT(DEC2HEX(L148), "00") &amp; IF(S148 &gt; 2, ", " &amp; "0x"&amp; TEXT(DEC2HEX(M148), "00") &amp; IF(S148 &gt; 3, ", " &amp; "0x"&amp; TEXT(DEC2HEX(N148), "00") &amp; IF(S148 &gt; 4, ", " &amp; "0x"&amp; TEXT(DEC2HEX(O148), "00") &amp; IF(S148 &gt; 5, ", " &amp; "0x"&amp; TEXT(DEC2HEX(P148), "00") &amp; IF(S148 &gt; 6, ", " &amp; "0x"&amp; TEXT(DEC2HEX(Q148), "00") &amp; IF(S148 &gt; 7, ", " &amp; "0x"&amp; TEXT(DEC2HEX(R148), "00"),),),),),),),),)</f>
-        <v>0x5C, 0x54, 0x74</v>
+        <v>0x58, 0x54, 0x34</v>
       </c>
       <c r="U148" s="12"/>
       <c r="V148" s="21"/>
@@ -13655,9 +13679,7 @@
     <row r="150" spans="1:25">
       <c r="A150" s="12"/>
       <c r="B150" s="72"/>
-      <c r="C150" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="C150" s="6"/>
       <c r="D150" s="5" t="s">
         <v>35</v>
       </c>
@@ -13785,9 +13807,7 @@
       <c r="D154" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E154" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="E154" s="5"/>
       <c r="F154" s="5"/>
       <c r="G154" s="5"/>
       <c r="H154" s="5"/>

</xml_diff>